<commit_message>
Changed From To postcode
</commit_message>
<xml_diff>
--- a/TestScenario_eCommerce.xlsx
+++ b/TestScenario_eCommerce.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FFE4A8-4AD2-47C9-ADDD-71CC3FC34350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4808962C-B17D-475E-A631-EBA826F97EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
   <si>
     <t>TS_001</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TS_015</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -590,6 +593,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -617,6 +626,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,18 +658,6 @@
     </xf>
     <xf numFmtId="15" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -997,8 +1003,8 @@
   </sheetPr>
   <dimension ref="B2:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35:G49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,50 +1021,50 @@
       <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="32"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="38">
         <v>43992</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="16"/>
     </row>
     <row r="8" spans="2:7" s="6" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1082,286 +1088,286 @@
       </c>
     </row>
     <row r="9" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="34" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="22">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:7" s="9" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
-      <c r="C11" s="29"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="21"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
-      <c r="C12" s="29"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="2:7" s="9" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
-      <c r="C13" s="29"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="2" t="s">
         <v>86</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="2:7" s="9" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
-      <c r="C14" s="29"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="21"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="30"/>
-      <c r="C15" s="29"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="21"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="30"/>
-      <c r="C16" s="29"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="21"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
-      <c r="C17" s="29"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="21"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
-      <c r="C18" s="29"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="21"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
-      <c r="C19" s="29"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="21"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="22"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="24"/>
     </row>
     <row r="21" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="25" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="21"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="21"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="22"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="24"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="34" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="22">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="30"/>
-      <c r="C26" s="29"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="21"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="30"/>
-      <c r="C27" s="29"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="21"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="30"/>
-      <c r="C28" s="29"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="21"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="23"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="30"/>
-      <c r="C29" s="29"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="34"/>
       <c r="D29" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="21"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="30"/>
-      <c r="C30" s="29"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="22"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="36" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="14"/>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G31" s="20">
+      <c r="G31" s="22">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="21"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="14" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="14"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="22"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
@@ -1374,7 +1380,7 @@
         <v>46</v>
       </c>
       <c r="E34" s="14"/>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="18" t="s">
         <v>96</v>
       </c>
       <c r="G34" s="8">
@@ -1382,178 +1388,178 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="25" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="35" t="s">
+      <c r="F35" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G35" s="20">
-        <v>11</v>
+      <c r="G35" s="22">
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="21"/>
-      <c r="C36" s="24"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="21"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="21"/>
-      <c r="C37" s="24"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="21"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="23"/>
     </row>
     <row r="38" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B38" s="21"/>
-      <c r="C38" s="24"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="26"/>
       <c r="D38" s="2" t="s">
         <v>52</v>
       </c>
       <c r="E38" s="2"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="21"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="21"/>
-      <c r="C39" s="24"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E39" s="2"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="21"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="21"/>
-      <c r="C40" s="24"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="26"/>
       <c r="D40" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="21"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B41" s="21"/>
-      <c r="C41" s="24"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="26"/>
       <c r="D41" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E41" s="2"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="21"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="21"/>
-      <c r="C42" s="24"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="26"/>
       <c r="D42" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="36"/>
-      <c r="G42" s="21"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
-      <c r="C43" s="24"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="26"/>
       <c r="D43" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="21"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="23"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="21"/>
-      <c r="C44" s="24"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="26"/>
       <c r="D44" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="21"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="23"/>
     </row>
     <row r="45" spans="2:7" s="15" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="21"/>
-      <c r="C45" s="24"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="26"/>
       <c r="D45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="21"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="23"/>
     </row>
     <row r="46" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
-      <c r="C46" s="24"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="26"/>
       <c r="D46" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="21"/>
-      <c r="C47" s="24"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="21"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="23"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="21"/>
-      <c r="C48" s="24"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="26"/>
       <c r="D48" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="21"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="23"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="22"/>
-      <c r="C49" s="25"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="22"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="33"/>
     </row>
     <row r="51" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>63</v>
@@ -1568,8 +1574,8 @@
       </c>
     </row>
     <row r="52" spans="2:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="8" t="s">
-        <v>67</v>
+      <c r="B52" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>79</v>
@@ -1584,8 +1590,8 @@
       </c>
     </row>
     <row r="53" spans="2:7" s="15" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="8" t="s">
-        <v>68</v>
+      <c r="B53" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>81</v>
@@ -1600,8 +1606,8 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B54" s="8" t="s">
-        <v>69</v>
+      <c r="B54" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>85</v>
@@ -1616,8 +1622,8 @@
       </c>
     </row>
     <row r="55" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B55" s="8" t="s">
-        <v>70</v>
+      <c r="B55" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>64</v>
@@ -1632,8 +1638,8 @@
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="8" t="s">
-        <v>71</v>
+      <c r="B56" s="17" t="s">
+        <v>72</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>65</v>
@@ -1648,8 +1654,8 @@
       </c>
     </row>
     <row r="57" spans="2:7" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B57" s="8" t="s">
-        <v>72</v>
+      <c r="B57" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>66</v>
@@ -1664,8 +1670,8 @@
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="8" t="s">
-        <v>80</v>
+      <c r="B58" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>77</v>
@@ -1680,8 +1686,8 @@
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="8" t="s">
-        <v>88</v>
+      <c r="B59" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>76</v>

</xml_diff>